<commit_message>
Definiting Bulwark::Import to centralize the import process. Defining new metadata source types for structural and descriptive metadata.
</commit_message>
<xml_diff>
--- a/spec/fixtures/example_manifest_loads/object_one_update/metadata.xlsx
+++ b/spec/fixtures/example_manifest_loads/object_one_update/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgalarza/code/bulwark/spec/fixtures/example_manifest_loads/object_one_update/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA339578-9C11-2846-BCC1-DED15DCDD057}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB3843A-74CD-E24E-B83A-E348720B5871}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8200" yWindow="1760" windowWidth="27640" windowHeight="16940" xr2:uid="{544C3912-5CC3-F541-A5DE-1377C76C530B}"/>
   </bookViews>
@@ -153,9 +153,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92148881-0C0D-484B-A289-7EE43A37FD2F}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -481,6 +482,7 @@
     <col min="2" max="2" width="17.83203125" customWidth="1"/>
     <col min="6" max="6" width="82.83203125" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="14" max="14" width="32.1640625" customWidth="1"/>
     <col min="15" max="15" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -577,7 +579,7 @@
       <c r="O2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="T2" s="1" t="s">

</xml_diff>